<commit_message>
Type in your commit message:
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="353">
   <si>
     <t>DATE</t>
   </si>
@@ -1048,6 +1048,33 @@
   </si>
   <si>
     <t>SX4</t>
+  </si>
+  <si>
+    <t>KA 03 MW 3617</t>
+  </si>
+  <si>
+    <t>XCENT</t>
+  </si>
+  <si>
+    <t>KA 51 MB 4552</t>
+  </si>
+  <si>
+    <t>SUSPENSION</t>
+  </si>
+  <si>
+    <t>KA 53 MD 9553</t>
+  </si>
+  <si>
+    <t>KL 01 CF 1995</t>
+  </si>
+  <si>
+    <t>KA 03 MT 2522</t>
+  </si>
+  <si>
+    <t>KA 53 MB 1800</t>
+  </si>
+  <si>
+    <t>SCALA</t>
   </si>
 </sst>
 </file>
@@ -1056,9 +1083,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="&quot;₹&quot;#,##0;&quot;₹&quot;\-#,##0"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
@@ -1071,15 +1098,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1093,22 +1114,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1117,22 +1131,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1161,6 +1159,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1185,6 +1190,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1200,7 +1227,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1208,8 +1234,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1224,7 +1251,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1236,13 +1263,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1260,67 +1341,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1344,7 +1377,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1356,25 +1389,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,25 +1419,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1415,41 +1442,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1501,6 +1493,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1515,19 +1533,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1536,130 +1563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2022,10 +2049,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G196"/>
+  <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="F197" sqref="F197"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -5816,6 +5843,126 @@
       </c>
       <c r="F196" s="3">
         <v>5546</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B197" t="s">
+        <v>344</v>
+      </c>
+      <c r="C197" t="s">
+        <v>345</v>
+      </c>
+      <c r="D197" t="s">
+        <v>138</v>
+      </c>
+      <c r="E197" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B198" t="s">
+        <v>346</v>
+      </c>
+      <c r="C198" t="s">
+        <v>18</v>
+      </c>
+      <c r="D198" t="s">
+        <v>347</v>
+      </c>
+      <c r="E198" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B199" t="s">
+        <v>348</v>
+      </c>
+      <c r="C199" t="s">
+        <v>281</v>
+      </c>
+      <c r="D199" t="s">
+        <v>90</v>
+      </c>
+      <c r="E199" t="s">
+        <v>28</v>
+      </c>
+      <c r="F199" s="3">
+        <v>2726</v>
+      </c>
+      <c r="G199" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B200" t="s">
+        <v>349</v>
+      </c>
+      <c r="C200" t="s">
+        <v>149</v>
+      </c>
+      <c r="D200" t="s">
+        <v>85</v>
+      </c>
+      <c r="E200" t="s">
+        <v>28</v>
+      </c>
+      <c r="F200" s="3">
+        <v>2360</v>
+      </c>
+      <c r="G200" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B201" t="s">
+        <v>350</v>
+      </c>
+      <c r="C201" t="s">
+        <v>163</v>
+      </c>
+      <c r="D201" t="s">
+        <v>37</v>
+      </c>
+      <c r="E201" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B202" t="s">
+        <v>351</v>
+      </c>
+      <c r="C202" t="s">
+        <v>352</v>
+      </c>
+      <c r="D202" t="s">
+        <v>85</v>
+      </c>
+      <c r="E202" t="s">
+        <v>28</v>
+      </c>
+      <c r="F202" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G202" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>